<commit_message>
worked on selectivity, up to Eq. (7)
</commit_message>
<xml_diff>
--- a/code/R/Selectivity parameters/BabcockRockfishInputs.xlsx
+++ b/code/R/Selectivity parameters/BabcockRockfishInputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vic\Documents\Projects\MS-thesis\code\R\Selectivity parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C4CB85-7833-4758-9666-D98DA21102DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC84088-4DB8-41D8-A374-2B1B3C7E0C26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13584" yWindow="288" windowWidth="5940" windowHeight="11736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8352" yWindow="0" windowWidth="7176" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BabcockRockfishInputs" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -710,6 +710,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -914,7 +920,6 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -923,6 +928,7 @@
     <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1281,7 +1287,7 @@
   <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2033,7 +2039,7 @@
       <c r="A38" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="10">
         <v>20</v>
       </c>
       <c r="C38">
@@ -2053,7 +2059,7 @@
       <c r="A39" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <v>0.45</v>
       </c>
       <c r="C39">
@@ -2073,7 +2079,7 @@
       <c r="A40" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="3">
         <v>25.2</v>
       </c>
       <c r="C40">
@@ -2093,7 +2099,7 @@
       <c r="A41" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="4">
         <v>31</v>
       </c>
       <c r="C41">
@@ -2113,7 +2119,7 @@
       <c r="A42" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="4">
         <v>29</v>
       </c>
       <c r="C42">
@@ -2133,7 +2139,7 @@
       <c r="A43" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="5">
         <v>1.28</v>
       </c>
       <c r="C43">
@@ -2153,7 +2159,7 @@
       <c r="A44" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="6">
         <v>36.700000000000003</v>
       </c>
       <c r="C44">
@@ -2173,7 +2179,7 @@
       <c r="A45" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="7">
         <v>0.26500000000000001</v>
       </c>
       <c r="C45">
@@ -2193,7 +2199,7 @@
       <c r="A46" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B46" s="8">
         <v>0.71</v>
       </c>
       <c r="C46">
@@ -2213,7 +2219,7 @@
       <c r="A47" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="9">
         <v>2</v>
       </c>
       <c r="C47">
@@ -2233,7 +2239,7 @@
       <c r="A48" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="10">
         <v>20</v>
       </c>
       <c r="C48">
@@ -2253,7 +2259,7 @@
       <c r="A49" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>0.36899999999999999</v>
       </c>
       <c r="C49">
@@ -2273,7 +2279,7 @@
       <c r="A50" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50" s="3">
         <v>33.200000000000003</v>
       </c>
       <c r="C50">
@@ -2293,7 +2299,7 @@
       <c r="A51" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="4">
         <v>39</v>
       </c>
       <c r="C51">
@@ -2313,7 +2319,7 @@
       <c r="A52" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="4">
         <v>29</v>
       </c>
       <c r="C52">
@@ -2333,7 +2339,7 @@
       <c r="A53" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53" s="5">
         <v>0.41899999999999998</v>
       </c>
       <c r="C53">
@@ -2353,7 +2359,7 @@
       <c r="A54" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B54" s="6">
         <v>46.4</v>
       </c>
       <c r="C54">
@@ -2373,7 +2379,7 @@
       <c r="A55" t="s">
         <v>59</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B55" s="7">
         <v>0.28999999999999998</v>
       </c>
       <c r="C55">
@@ -2393,7 +2399,7 @@
       <c r="A56" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="9">
+      <c r="B56" s="8">
         <v>0.28000000000000003</v>
       </c>
       <c r="C56">
@@ -2413,7 +2419,7 @@
       <c r="A57" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="10">
+      <c r="B57" s="9">
         <v>1</v>
       </c>
       <c r="C57">
@@ -2433,7 +2439,7 @@
       <c r="A58" t="s">
         <v>62</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="10">
         <v>20</v>
       </c>
       <c r="C58">
@@ -2453,7 +2459,7 @@
       <c r="A59" t="s">
         <v>63</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="2">
         <v>0.42599999999999999</v>
       </c>
       <c r="C59">
@@ -2473,7 +2479,7 @@
       <c r="A60" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="4">
+      <c r="B60" s="3">
         <v>46</v>
       </c>
       <c r="C60">
@@ -2493,7 +2499,7 @@
       <c r="A61" t="s">
         <v>65</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B61" s="4">
         <v>0</v>
       </c>
       <c r="C61">
@@ -2513,7 +2519,7 @@
       <c r="A62" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="5">
+      <c r="B62" s="4">
         <v>0</v>
       </c>
       <c r="C62">
@@ -2533,7 +2539,7 @@
       <c r="A63" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63" s="5">
         <v>0</v>
       </c>
       <c r="C63">
@@ -2553,7 +2559,7 @@
       <c r="A64" t="s">
         <v>68</v>
       </c>
-      <c r="B64" s="7">
+      <c r="B64" s="6">
         <v>50</v>
       </c>
       <c r="C64">
@@ -2573,7 +2579,7 @@
       <c r="A65" t="s">
         <v>69</v>
       </c>
-      <c r="B65" s="8">
+      <c r="B65" s="7">
         <v>0</v>
       </c>
       <c r="C65">
@@ -2593,7 +2599,7 @@
       <c r="A66" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="9">
+      <c r="B66" s="8">
         <v>0.01</v>
       </c>
       <c r="C66">
@@ -2613,7 +2619,7 @@
       <c r="A67" t="s">
         <v>71</v>
       </c>
-      <c r="B67" s="10">
+      <c r="B67" s="9">
         <v>1</v>
       </c>
       <c r="C67">

</xml_diff>